<commit_message>
Upload revised 2020 excel file and create dates
</commit_message>
<xml_diff>
--- a/data/Buddy_Bass_Tournament_2020.xlsx
+++ b/data/Buddy_Bass_Tournament_2020.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mh3Q3mf2/qzkK0qaMNlePAW+LoOqQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgCKJKAPZebyeCs4ZsTVPQgYpZZsg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -802,48 +802,48 @@
       <c r="H15" s="24"/>
     </row>
     <row r="16" ht="23.25" customHeight="1">
-      <c r="A16" s="20">
-        <v>44087.0</v>
-      </c>
-      <c r="B16" s="21">
-        <v>27.0</v>
-      </c>
-      <c r="C16" s="17">
-        <v>84.0</v>
-      </c>
-      <c r="D16" s="22">
-        <v>125.42</v>
-      </c>
-      <c r="E16" s="17">
-        <v>4.28</v>
-      </c>
-      <c r="F16" s="17">
-        <v>78.8</v>
-      </c>
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="23"/>
       <c r="H16" s="24"/>
     </row>
     <row r="17" ht="23.25" customHeight="1">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="15"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="24"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="15"/>
+    <row r="18" ht="23.25" customHeight="1">
+      <c r="A18" s="20">
+        <v>44087.0</v>
+      </c>
+      <c r="B18" s="21">
+        <v>27.0</v>
+      </c>
+      <c r="C18" s="17">
+        <v>84.0</v>
+      </c>
+      <c r="D18" s="22">
+        <v>125.42</v>
+      </c>
+      <c r="E18" s="17">
+        <v>4.28</v>
+      </c>
+      <c r="F18" s="17">
+        <v>78.8</v>
+      </c>
+      <c r="G18" s="23"/>
       <c r="H18" s="24"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" ht="23.25" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="25"/>
       <c r="C19" s="24"/>
@@ -2120,7 +2120,7 @@
       <c r="D146" s="24"/>
       <c r="E146" s="24"/>
       <c r="F146" s="24"/>
-      <c r="G146" s="24"/>
+      <c r="G146" s="15"/>
       <c r="H146" s="24"/>
     </row>
     <row r="147" ht="14.25" customHeight="1">
@@ -2130,7 +2130,7 @@
       <c r="D147" s="24"/>
       <c r="E147" s="24"/>
       <c r="F147" s="24"/>
-      <c r="G147" s="24"/>
+      <c r="G147" s="15"/>
       <c r="H147" s="24"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
@@ -2834,10 +2834,24 @@
       <c r="H217" s="24"/>
     </row>
     <row r="218" ht="14.25" customHeight="1">
-      <c r="B218" s="26"/>
+      <c r="A218" s="24"/>
+      <c r="B218" s="25"/>
+      <c r="C218" s="24"/>
+      <c r="D218" s="24"/>
+      <c r="E218" s="24"/>
+      <c r="F218" s="24"/>
+      <c r="G218" s="24"/>
+      <c r="H218" s="24"/>
     </row>
     <row r="219" ht="14.25" customHeight="1">
-      <c r="B219" s="26"/>
+      <c r="A219" s="24"/>
+      <c r="B219" s="25"/>
+      <c r="C219" s="24"/>
+      <c r="D219" s="24"/>
+      <c r="E219" s="24"/>
+      <c r="F219" s="24"/>
+      <c r="G219" s="24"/>
+      <c r="H219" s="24"/>
     </row>
     <row r="220" ht="14.25" customHeight="1">
       <c r="B220" s="26"/>
@@ -5116,8 +5130,12 @@
     <row r="978" ht="14.25" customHeight="1">
       <c r="B978" s="26"/>
     </row>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
+    <row r="979" ht="14.25" customHeight="1">
+      <c r="B979" s="26"/>
+    </row>
+    <row r="980" ht="14.25" customHeight="1">
+      <c r="B980" s="26"/>
+    </row>
     <row r="981" ht="14.25" customHeight="1"/>
     <row r="982" ht="14.25" customHeight="1"/>
     <row r="983" ht="14.25" customHeight="1"/>
@@ -5127,6 +5145,8 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>

</xml_diff>